<commit_message>
feat: day 24 part b
</commit_message>
<xml_diff>
--- a/src/day-24/calcoli.xlsx
+++ b/src/day-24/calcoli.xlsx
@@ -8,27 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francesco/sviluppo/git/advent-of-code-2021/src/day-24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34249FDA-69E1-1E41-8976-61B3D148C077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467A7C08-89BE-764C-AB00-3889A2E34D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="1520" windowWidth="28040" windowHeight="17440" xr2:uid="{5419EF10-27CC-0A4B-991C-55FD0045AB79}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Foglio1!$A$2:$A$15</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Foglio1!$B$2:$B$15</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Foglio1!$C$2:$C$15</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Foglio1!$A$2:$A$15</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Foglio1!$B$2:$B$15</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Foglio1!$C$2:$C$15</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Foglio1!$A$2:$A$15</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Foglio1!$B$2:$B$15</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Foglio1!$C$2:$C$15</definedName>
-    <definedName name="_xlchart.v2.10" hidden="1">Foglio1!$B$2:$B$15</definedName>
-    <definedName name="_xlchart.v2.11" hidden="1">Foglio1!$C$2:$C$15</definedName>
-    <definedName name="_xlchart.v2.9" hidden="1">Foglio1!$A$2:$A$15</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -48,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
     <t>input</t>
   </si>
@@ -74,13 +60,19 @@
     <t>modZ+addX</t>
   </si>
   <si>
-    <t>deve essere 9 + addY precedente - addX</t>
+    <t>x</t>
   </si>
   <si>
-    <t>deve essere 9 + addY di posizione 8 - addX o al minimo 9</t>
+    <t>deve essere 9 + addY precedente + addX</t>
   </si>
   <si>
-    <t>x</t>
+    <t>deve essere 9 + addY di posizione 8 + addX o al minimo 9</t>
+  </si>
+  <si>
+    <t>deve essere il massimo fra 1 e 1 + addY precedente + addX</t>
+  </si>
+  <si>
+    <t>deve essere il massimo fra 1 e 1 + addY di posizione 8 + addX</t>
   </si>
 </sst>
 </file>
@@ -432,13 +424,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{594EAA46-1E23-4D44-B360-961D934A2C9F}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -493,7 +488,7 @@
         <v>17</v>
       </c>
       <c r="O2">
-        <f>B12 - D12 - E2</f>
+        <f>B13 - D13 - E2</f>
         <v>5</v>
       </c>
     </row>
@@ -625,14 +620,14 @@
         <v>11947</v>
       </c>
       <c r="J6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O6">
         <f>MIN(9,9+E5+D6)</f>
         <v>2</v>
       </c>
       <c r="P6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -697,14 +692,14 @@
         <v>11947</v>
       </c>
       <c r="J8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O8">
         <f>MIN(9,9+E7+D8)</f>
         <v>9</v>
       </c>
       <c r="P8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -769,14 +764,14 @@
         <v>11947</v>
       </c>
       <c r="J10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O10">
         <f>MIN(9,9+E9+D10)</f>
         <v>9</v>
       </c>
       <c r="P10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -808,14 +803,14 @@
         <v>459</v>
       </c>
       <c r="J11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O11">
-        <f>MIN(9,9+E9+D11)</f>
+        <f>MIN(9,9+E4+D11)</f>
         <v>9</v>
       </c>
       <c r="P11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -847,14 +842,14 @@
         <v>17</v>
       </c>
       <c r="J12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O12">
-        <f>MIN(9,9+E9+D12)</f>
+        <f>MIN(9,9+E3+D12)</f>
         <v>4</v>
       </c>
       <c r="P12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -886,14 +881,14 @@
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O13">
-        <f>MIN(9,9+E9+D13)</f>
+        <f>MIN(9,9+E2+D13)</f>
         <v>9</v>
       </c>
       <c r="P13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
@@ -958,14 +953,495 @@
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O15">
         <f>MIN(9,9+E14+D15)</f>
         <v>8</v>
       </c>
       <c r="P15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>14</v>
+      </c>
+      <c r="E18">
+        <v>12</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f>B18+E18</f>
+        <v>13</v>
+      </c>
+      <c r="O18">
+        <f>B29 - D29 - E18</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>11</v>
+      </c>
+      <c r="E19">
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <f>MOD(H18,26)</f>
+        <v>13</v>
+      </c>
+      <c r="G19">
+        <f>F19 + D19</f>
+        <v>24</v>
+      </c>
+      <c r="H19">
+        <f t="shared" ref="H19:H21" si="4">IF(G19=B19,TRUNC(H18/26),H18 * 26 + B19 + E19)</f>
+        <v>352</v>
+      </c>
+      <c r="O19">
+        <f>B28 - D28 - E19</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>11</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ref="F20:F31" si="5">MOD(H19,26)</f>
+        <v>14</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ref="G20:G31" si="6">F20 + D20</f>
+        <v>25</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="4"/>
+        <v>9160</v>
+      </c>
+      <c r="O20">
+        <f>B27 - D27 - E20</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>14</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="6"/>
+        <v>22</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="4"/>
+        <v>238172</v>
+      </c>
+      <c r="O21">
+        <f>B22-D22-E21</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>26</v>
+      </c>
+      <c r="D22">
+        <v>-11</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <f>IF(G22=B22,TRUNC(H21/26),H21 * 26 + B22 + E22)</f>
+        <v>9160</v>
+      </c>
+      <c r="J22" t="s">
+        <v>11</v>
+      </c>
+      <c r="O22">
+        <f>MAX(1,1+E21+D22)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>12</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="H23">
+        <f t="shared" ref="H23:H31" si="7">IF(G23=B23,TRUNC(H22/26),H22 * 26 + B23 + E23)</f>
+        <v>238162</v>
+      </c>
+      <c r="O23">
+        <f>B24-D24-E23</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>26</v>
+      </c>
+      <c r="D24">
+        <v>-1</v>
+      </c>
+      <c r="E24">
         <v>10</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="7"/>
+        <v>9160</v>
+      </c>
+      <c r="J24" t="s">
+        <v>11</v>
+      </c>
+      <c r="O24">
+        <f>MAX(1,1+E23+D24)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="E25">
+        <v>8</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="7"/>
+        <v>238169</v>
+      </c>
+      <c r="O25">
+        <f>B26-D26-E25</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>26</v>
+      </c>
+      <c r="D26">
+        <v>-3</v>
+      </c>
+      <c r="E26">
+        <v>12</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="7"/>
+        <v>9160</v>
+      </c>
+      <c r="J26" t="s">
+        <v>12</v>
+      </c>
+      <c r="O26">
+        <f>MAX(1,1+E25+D26)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>26</v>
+      </c>
+      <c r="D27">
+        <v>-4</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="7"/>
+        <v>352</v>
+      </c>
+      <c r="J27" t="s">
+        <v>12</v>
+      </c>
+      <c r="O27">
+        <f>MAX(1,1+E20+D27)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>11</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>26</v>
+      </c>
+      <c r="D28">
+        <v>-13</v>
+      </c>
+      <c r="E28">
+        <v>15</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="J28" t="s">
+        <v>12</v>
+      </c>
+      <c r="O28">
+        <f>MAX(1,1+E19+D28)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>12</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>26</v>
+      </c>
+      <c r="D29">
+        <v>-8</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J29" t="s">
+        <v>12</v>
+      </c>
+      <c r="O29">
+        <f>MAX(1,1+E18+D29)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>13</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>13</v>
+      </c>
+      <c r="E30">
+        <v>10</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="O30">
+        <f>B31-D31-E30</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>14</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>26</v>
+      </c>
+      <c r="D31">
+        <v>-11</v>
+      </c>
+      <c r="E31">
+        <v>9</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J31" t="s">
+        <v>11</v>
+      </c>
+      <c r="O31">
+        <f>MAX(1,1+E30+D31)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>